<commit_message>
You Are What YOu Eat Final Uploaded
</commit_message>
<xml_diff>
--- a/WWW/posts/you-are-what-you-eat/post_info.xlsx
+++ b/WWW/posts/you-are-what-you-eat/post_info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="403" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>The Dish on Science</t>
   </si>
@@ -62,7 +62,7 @@
     <t>5x2 (WxH) Image File Name</t>
   </si>
   <si>
-    <t>./images/tdos_youarewhatyoueat_dairycows.jpeg</t>
+    <t>./images/tdos_youarewhatyoueat_dairycowsnew.jpeg</t>
   </si>
   <si>
     <t>Post Blurb</t>
@@ -77,7 +77,7 @@
     <t>Post Description</t>
   </si>
   <si>
-    <t>We know that the planet is slowly dying, but what you might not know is how much your weekly cheeseburger is contributing to not only greenhouse gas emissions but also water and land depletion. </t>
+    <t>We know that the planet is slowly dying, but what you might not know is how much your weekly cheeseburger is contributing to not only greenhouse gas emissions but also water and land depletion.</t>
   </si>
   <si>
     <t>thedishonscience.stanford.edu/topics/USE-THIS-STRING</t>
@@ -132,17 +132,15 @@
   </si>
   <si>
     <t>1x1 (WxH) Image File Name (Thumbnail)</t>
-  </si>
-  <si>
-    <t>2019/11/06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -301,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,6 +377,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,15 +461,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>112680</xdr:colOff>
+      <xdr:colOff>139680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>617040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>216360</xdr:rowOff>
+      <xdr:colOff>643680</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>219600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -480,8 +482,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="112680" y="38520"/>
-          <a:ext cx="504360" cy="571320"/>
+          <a:off x="139680" y="29520"/>
+          <a:ext cx="504000" cy="570960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -503,21 +505,21 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.17004048583"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.4331983805668"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -528,7 +530,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -550,7 +552,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -569,7 +571,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
         <v>4</v>
@@ -599,7 +601,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="12" t="s">
         <v>10</v>
@@ -614,7 +616,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="128" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>13</v>
@@ -767,7 +769,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="12" t="s">
         <v>37</v>
@@ -784,8 +786,8 @@
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>39</v>
+      <c r="D21" s="20" t="n">
+        <v>43777</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>

</xml_diff>